<commit_message>
menambahkan etalase export excel dan import produk dengan etalase id
</commit_message>
<xml_diff>
--- a/storage/Dokumen/Doc-20200418.xlsx
+++ b/storage/Dokumen/Doc-20200418.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Foto</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Kategori ID</t>
+  </si>
+  <si>
+    <t>Etalase ID</t>
   </si>
   <si>
     <t>Kondisi (Baru/Bekas)</t>
@@ -74,8 +77,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -105,6 +108,14 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -116,6 +127,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,6 +142,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -132,20 +159,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -153,70 +180,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,6 +209,29 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -239,43 +242,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,37 +386,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,25 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,67 +416,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,6 +433,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -452,22 +475,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,19 +498,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,162 +533,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -866,7 +869,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -890,9 +893,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -916,7 +919,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -969,7 +972,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -994,7 +997,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1006,27 +1009,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="19.75" customWidth="1"/>
-    <col min="5" max="5" width="28.875" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
-    <col min="7" max="7" width="16.625" customWidth="1"/>
-    <col min="8" max="8" width="22.375" customWidth="1"/>
-    <col min="10" max="10" width="27.375" customWidth="1"/>
-    <col min="11" max="11" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="true"/>
+    <col min="2" max="2" width="23.5" customWidth="true"/>
+    <col min="3" max="4" width="10.625" customWidth="true"/>
+    <col min="5" max="5" width="19.75" customWidth="true"/>
+    <col min="6" max="6" width="28.875" customWidth="true"/>
+    <col min="7" max="7" width="19.875" customWidth="true"/>
+    <col min="8" max="8" width="16.625" customWidth="true"/>
+    <col min="9" max="9" width="22.375" customWidth="true"/>
+    <col min="11" max="11" width="27.375" customWidth="true"/>
+    <col min="12" max="12" width="12.375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1060,39 +1063,45 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1000</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2">
         <v>100</v>
       </c>
     </row>

</xml_diff>